<commit_message>
modificaciones en los atributos de la clase datos
</commit_message>
<xml_diff>
--- a/Documentación/Cronograma.xlsx
+++ b/Documentación/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52646\Desktop\ProyectoBDITE\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6FA43F-C2A7-4E38-9FFD-055D22F5C0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3489832E-C15F-4AE3-93F9-983B838D7ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{77C97420-D882-4AEC-80C4-94E9F25F4DD9}"/>
   </bookViews>
@@ -945,6 +945,15 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -954,25 +963,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770ABD26-0474-45FB-9EFD-7F425FDDCB3A}">
   <dimension ref="A1:EF56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,130 +1342,130 @@
       <c r="E1" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="70" t="s">
+      <c r="O1" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="70"/>
-      <c r="AL1" s="70"/>
-      <c r="AM1" s="70"/>
-      <c r="AN1" s="70"/>
-      <c r="AO1" s="70"/>
-      <c r="AP1" s="70"/>
-      <c r="AQ1" s="70"/>
-      <c r="AR1" s="70"/>
-      <c r="AS1" s="70"/>
-      <c r="AT1" s="70"/>
-      <c r="AU1" s="70"/>
-      <c r="AV1" s="70"/>
-      <c r="AW1" s="70"/>
-      <c r="AX1" s="70"/>
-      <c r="AY1" s="70"/>
-      <c r="AZ1" s="70"/>
-      <c r="BA1" s="70"/>
-      <c r="BB1" s="70"/>
-      <c r="BC1" s="70"/>
-      <c r="BD1" s="70"/>
-      <c r="BE1" s="70"/>
-      <c r="BF1" s="70"/>
-      <c r="BG1" s="70"/>
-      <c r="BH1" s="70"/>
-      <c r="BI1" s="70"/>
-      <c r="BJ1" s="70"/>
-      <c r="BK1" s="70"/>
-      <c r="BL1" s="70"/>
-      <c r="BM1" s="70"/>
-      <c r="BN1" s="70"/>
-      <c r="BO1" s="70"/>
-      <c r="BP1" s="70"/>
-      <c r="BQ1" s="70"/>
-      <c r="BR1" s="70"/>
-      <c r="BS1" s="70"/>
-      <c r="BT1" s="70"/>
-      <c r="BU1" s="70"/>
-      <c r="BV1" s="70"/>
-      <c r="BW1" s="70"/>
-      <c r="BX1" s="70"/>
-      <c r="BY1" s="70"/>
-      <c r="BZ1" s="70"/>
-      <c r="CA1" s="70"/>
-      <c r="CB1" s="70"/>
-      <c r="CC1" s="70"/>
-      <c r="CD1" s="70"/>
-      <c r="CE1" s="70"/>
-      <c r="CF1" s="70"/>
-      <c r="CG1" s="70"/>
-      <c r="CH1" s="70"/>
-      <c r="CI1" s="70"/>
-      <c r="CJ1" s="70"/>
-      <c r="CK1" s="70"/>
-      <c r="CL1" s="70"/>
-      <c r="CM1" s="70"/>
-      <c r="CN1" s="70"/>
-      <c r="CO1" s="70"/>
-      <c r="CP1" s="70"/>
-      <c r="CQ1" s="70"/>
-      <c r="CR1" s="70"/>
-      <c r="CS1" s="70"/>
-      <c r="CT1" s="70"/>
-      <c r="CU1" s="70"/>
-      <c r="CV1" s="70"/>
-      <c r="CW1" s="70"/>
-      <c r="CX1" s="70"/>
-      <c r="CY1" s="70"/>
-      <c r="CZ1" s="70"/>
-      <c r="DA1" s="70"/>
-      <c r="DB1" s="70"/>
-      <c r="DC1" s="70"/>
-      <c r="DD1" s="70"/>
-      <c r="DE1" s="70"/>
-      <c r="DF1" s="70"/>
-      <c r="DG1" s="70"/>
-      <c r="DH1" s="70"/>
-      <c r="DI1" s="70"/>
-      <c r="DJ1" s="70"/>
-      <c r="DK1" s="70"/>
-      <c r="DL1" s="70"/>
-      <c r="DM1" s="70"/>
-      <c r="DN1" s="70"/>
-      <c r="DO1" s="70"/>
-      <c r="DP1" s="70"/>
-      <c r="DQ1" s="70"/>
-      <c r="DR1" s="70"/>
-      <c r="DS1" s="70"/>
-      <c r="DT1" s="70"/>
-      <c r="DU1" s="70"/>
-      <c r="DV1" s="70"/>
-      <c r="DW1" s="70"/>
-      <c r="DX1" s="70"/>
-      <c r="DY1" s="70"/>
-      <c r="DZ1" s="70"/>
-      <c r="EA1" s="70"/>
-      <c r="EB1" s="70"/>
-      <c r="EC1" s="70"/>
-      <c r="ED1" s="70"/>
-      <c r="EE1" s="70"/>
-      <c r="EF1" s="70"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="75"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="75"/>
+      <c r="AG1" s="75"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="75"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="75"/>
+      <c r="AM1" s="75"/>
+      <c r="AN1" s="75"/>
+      <c r="AO1" s="75"/>
+      <c r="AP1" s="75"/>
+      <c r="AQ1" s="75"/>
+      <c r="AR1" s="75"/>
+      <c r="AS1" s="75"/>
+      <c r="AT1" s="75"/>
+      <c r="AU1" s="75"/>
+      <c r="AV1" s="75"/>
+      <c r="AW1" s="75"/>
+      <c r="AX1" s="75"/>
+      <c r="AY1" s="75"/>
+      <c r="AZ1" s="75"/>
+      <c r="BA1" s="75"/>
+      <c r="BB1" s="75"/>
+      <c r="BC1" s="75"/>
+      <c r="BD1" s="75"/>
+      <c r="BE1" s="75"/>
+      <c r="BF1" s="75"/>
+      <c r="BG1" s="75"/>
+      <c r="BH1" s="75"/>
+      <c r="BI1" s="75"/>
+      <c r="BJ1" s="75"/>
+      <c r="BK1" s="75"/>
+      <c r="BL1" s="75"/>
+      <c r="BM1" s="75"/>
+      <c r="BN1" s="75"/>
+      <c r="BO1" s="75"/>
+      <c r="BP1" s="75"/>
+      <c r="BQ1" s="75"/>
+      <c r="BR1" s="75"/>
+      <c r="BS1" s="75"/>
+      <c r="BT1" s="75"/>
+      <c r="BU1" s="75"/>
+      <c r="BV1" s="75"/>
+      <c r="BW1" s="75"/>
+      <c r="BX1" s="75"/>
+      <c r="BY1" s="75"/>
+      <c r="BZ1" s="75"/>
+      <c r="CA1" s="75"/>
+      <c r="CB1" s="75"/>
+      <c r="CC1" s="75"/>
+      <c r="CD1" s="75"/>
+      <c r="CE1" s="75"/>
+      <c r="CF1" s="75"/>
+      <c r="CG1" s="75"/>
+      <c r="CH1" s="75"/>
+      <c r="CI1" s="75"/>
+      <c r="CJ1" s="75"/>
+      <c r="CK1" s="75"/>
+      <c r="CL1" s="75"/>
+      <c r="CM1" s="75"/>
+      <c r="CN1" s="75"/>
+      <c r="CO1" s="75"/>
+      <c r="CP1" s="75"/>
+      <c r="CQ1" s="75"/>
+      <c r="CR1" s="75"/>
+      <c r="CS1" s="75"/>
+      <c r="CT1" s="75"/>
+      <c r="CU1" s="75"/>
+      <c r="CV1" s="75"/>
+      <c r="CW1" s="75"/>
+      <c r="CX1" s="75"/>
+      <c r="CY1" s="75"/>
+      <c r="CZ1" s="75"/>
+      <c r="DA1" s="75"/>
+      <c r="DB1" s="75"/>
+      <c r="DC1" s="75"/>
+      <c r="DD1" s="75"/>
+      <c r="DE1" s="75"/>
+      <c r="DF1" s="75"/>
+      <c r="DG1" s="75"/>
+      <c r="DH1" s="75"/>
+      <c r="DI1" s="75"/>
+      <c r="DJ1" s="75"/>
+      <c r="DK1" s="75"/>
+      <c r="DL1" s="75"/>
+      <c r="DM1" s="75"/>
+      <c r="DN1" s="75"/>
+      <c r="DO1" s="75"/>
+      <c r="DP1" s="75"/>
+      <c r="DQ1" s="75"/>
+      <c r="DR1" s="75"/>
+      <c r="DS1" s="75"/>
+      <c r="DT1" s="75"/>
+      <c r="DU1" s="75"/>
+      <c r="DV1" s="75"/>
+      <c r="DW1" s="75"/>
+      <c r="DX1" s="75"/>
+      <c r="DY1" s="75"/>
+      <c r="DZ1" s="75"/>
+      <c r="EA1" s="75"/>
+      <c r="EB1" s="75"/>
+      <c r="EC1" s="75"/>
+      <c r="ED1" s="75"/>
+      <c r="EE1" s="75"/>
+      <c r="EF1" s="75"/>
     </row>
     <row r="2" spans="1:136" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
@@ -1477,94 +1477,94 @@
       <c r="C2" s="9"/>
       <c r="D2" s="10"/>
       <c r="E2" s="11"/>
-      <c r="I2" s="72" t="s">
+      <c r="I2" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="73"/>
-      <c r="AC2" s="69" t="s">
+      <c r="J2" s="68"/>
+      <c r="AC2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="AD2" s="69"/>
-      <c r="AE2" s="69"/>
-      <c r="AF2" s="69"/>
-      <c r="AG2" s="69"/>
-      <c r="AH2" s="69"/>
-      <c r="AI2" s="69"/>
-      <c r="AJ2" s="69"/>
-      <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
-      <c r="AM2" s="69"/>
-      <c r="AN2" s="69"/>
-      <c r="AO2" s="69"/>
-      <c r="AP2" s="69"/>
-      <c r="AQ2" s="69"/>
-      <c r="AR2" s="69"/>
-      <c r="AS2" s="69"/>
-      <c r="AT2" s="74" t="s">
+      <c r="AD2" s="74"/>
+      <c r="AE2" s="74"/>
+      <c r="AF2" s="74"/>
+      <c r="AG2" s="74"/>
+      <c r="AH2" s="74"/>
+      <c r="AI2" s="74"/>
+      <c r="AJ2" s="74"/>
+      <c r="AK2" s="74"/>
+      <c r="AL2" s="74"/>
+      <c r="AM2" s="74"/>
+      <c r="AN2" s="74"/>
+      <c r="AO2" s="74"/>
+      <c r="AP2" s="74"/>
+      <c r="AQ2" s="74"/>
+      <c r="AR2" s="74"/>
+      <c r="AS2" s="74"/>
+      <c r="AT2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="AU2" s="74"/>
-      <c r="AV2" s="74"/>
-      <c r="AW2" s="74"/>
-      <c r="AX2" s="74"/>
-      <c r="AY2" s="74"/>
-      <c r="AZ2" s="74"/>
-      <c r="BA2" s="74"/>
-      <c r="BB2" s="74"/>
-      <c r="BC2" s="74"/>
-      <c r="BD2" s="74"/>
-      <c r="BE2" s="74"/>
-      <c r="BF2" s="74"/>
-      <c r="BG2" s="74"/>
-      <c r="BH2" s="74"/>
-      <c r="BI2" s="74"/>
-      <c r="BJ2" s="74"/>
-      <c r="BK2" s="74"/>
-      <c r="BL2" s="74"/>
-      <c r="BM2" s="74"/>
-      <c r="BN2" s="74"/>
-      <c r="BO2" s="74"/>
-      <c r="BP2" s="74"/>
-      <c r="BQ2" s="74"/>
-      <c r="BR2" s="74"/>
-      <c r="BS2" s="74"/>
-      <c r="BT2" s="74"/>
-      <c r="BU2" s="74"/>
-      <c r="BV2" s="74"/>
-      <c r="BW2" s="74"/>
-      <c r="BX2" s="75" t="s">
+      <c r="AU2" s="72"/>
+      <c r="AV2" s="72"/>
+      <c r="AW2" s="72"/>
+      <c r="AX2" s="72"/>
+      <c r="AY2" s="72"/>
+      <c r="AZ2" s="72"/>
+      <c r="BA2" s="72"/>
+      <c r="BB2" s="72"/>
+      <c r="BC2" s="72"/>
+      <c r="BD2" s="72"/>
+      <c r="BE2" s="72"/>
+      <c r="BF2" s="72"/>
+      <c r="BG2" s="72"/>
+      <c r="BH2" s="72"/>
+      <c r="BI2" s="72"/>
+      <c r="BJ2" s="72"/>
+      <c r="BK2" s="72"/>
+      <c r="BL2" s="72"/>
+      <c r="BM2" s="72"/>
+      <c r="BN2" s="72"/>
+      <c r="BO2" s="72"/>
+      <c r="BP2" s="72"/>
+      <c r="BQ2" s="72"/>
+      <c r="BR2" s="72"/>
+      <c r="BS2" s="72"/>
+      <c r="BT2" s="72"/>
+      <c r="BU2" s="72"/>
+      <c r="BV2" s="72"/>
+      <c r="BW2" s="72"/>
+      <c r="BX2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="BY2" s="75"/>
-      <c r="BZ2" s="75"/>
-      <c r="CA2" s="75"/>
-      <c r="CB2" s="75"/>
-      <c r="CC2" s="75"/>
-      <c r="CD2" s="75"/>
-      <c r="CE2" s="75"/>
-      <c r="CF2" s="75"/>
-      <c r="CG2" s="75"/>
-      <c r="CH2" s="75"/>
-      <c r="CI2" s="75"/>
-      <c r="CJ2" s="75"/>
-      <c r="CK2" s="75"/>
-      <c r="CL2" s="75"/>
-      <c r="CM2" s="75"/>
-      <c r="CN2" s="75"/>
-      <c r="CO2" s="75"/>
-      <c r="CP2" s="75"/>
-      <c r="CQ2" s="75"/>
-      <c r="CR2" s="75"/>
-      <c r="CS2" s="75"/>
-      <c r="CT2" s="75"/>
-      <c r="CU2" s="75"/>
-      <c r="CV2" s="75"/>
-      <c r="CW2" s="75"/>
-      <c r="CX2" s="75"/>
-      <c r="CY2" s="75"/>
-      <c r="CZ2" s="75"/>
-      <c r="DA2" s="75"/>
-      <c r="DB2" s="75"/>
+      <c r="BY2" s="73"/>
+      <c r="BZ2" s="73"/>
+      <c r="CA2" s="73"/>
+      <c r="CB2" s="73"/>
+      <c r="CC2" s="73"/>
+      <c r="CD2" s="73"/>
+      <c r="CE2" s="73"/>
+      <c r="CF2" s="73"/>
+      <c r="CG2" s="73"/>
+      <c r="CH2" s="73"/>
+      <c r="CI2" s="73"/>
+      <c r="CJ2" s="73"/>
+      <c r="CK2" s="73"/>
+      <c r="CL2" s="73"/>
+      <c r="CM2" s="73"/>
+      <c r="CN2" s="73"/>
+      <c r="CO2" s="73"/>
+      <c r="CP2" s="73"/>
+      <c r="CQ2" s="73"/>
+      <c r="CR2" s="73"/>
+      <c r="CS2" s="73"/>
+      <c r="CT2" s="73"/>
+      <c r="CU2" s="73"/>
+      <c r="CV2" s="73"/>
+      <c r="CW2" s="73"/>
+      <c r="CX2" s="73"/>
+      <c r="CY2" s="73"/>
+      <c r="CZ2" s="73"/>
+      <c r="DA2" s="73"/>
+      <c r="DB2" s="73"/>
       <c r="DC2" s="76" t="s">
         <v>3</v>
       </c>
@@ -1591,117 +1591,117 @@
       <c r="E3" s="5"/>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
-      <c r="AC3" s="66" t="s">
+      <c r="AC3" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="67"/>
-      <c r="AH3" s="67"/>
-      <c r="AI3" s="68"/>
-      <c r="AJ3" s="67" t="s">
+      <c r="AD3" s="70"/>
+      <c r="AE3" s="70"/>
+      <c r="AF3" s="70"/>
+      <c r="AG3" s="70"/>
+      <c r="AH3" s="70"/>
+      <c r="AI3" s="71"/>
+      <c r="AJ3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="AK3" s="67"/>
-      <c r="AL3" s="67"/>
-      <c r="AM3" s="67"/>
-      <c r="AN3" s="67"/>
-      <c r="AO3" s="67"/>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="67"/>
-      <c r="AR3" s="67"/>
-      <c r="AS3" s="68"/>
-      <c r="AT3" s="66" t="s">
+      <c r="AK3" s="70"/>
+      <c r="AL3" s="70"/>
+      <c r="AM3" s="70"/>
+      <c r="AN3" s="70"/>
+      <c r="AO3" s="70"/>
+      <c r="AP3" s="70"/>
+      <c r="AQ3" s="70"/>
+      <c r="AR3" s="70"/>
+      <c r="AS3" s="71"/>
+      <c r="AT3" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="AU3" s="67"/>
-      <c r="AV3" s="67"/>
-      <c r="AW3" s="67"/>
-      <c r="AX3" s="67"/>
-      <c r="AY3" s="67"/>
-      <c r="AZ3" s="67"/>
-      <c r="BA3" s="67"/>
-      <c r="BB3" s="68"/>
-      <c r="BC3" s="66" t="s">
+      <c r="AU3" s="70"/>
+      <c r="AV3" s="70"/>
+      <c r="AW3" s="70"/>
+      <c r="AX3" s="70"/>
+      <c r="AY3" s="70"/>
+      <c r="AZ3" s="70"/>
+      <c r="BA3" s="70"/>
+      <c r="BB3" s="71"/>
+      <c r="BC3" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="BD3" s="67"/>
-      <c r="BE3" s="67"/>
-      <c r="BF3" s="67"/>
-      <c r="BG3" s="67"/>
-      <c r="BH3" s="67"/>
-      <c r="BI3" s="68"/>
-      <c r="BJ3" s="66" t="s">
+      <c r="BD3" s="70"/>
+      <c r="BE3" s="70"/>
+      <c r="BF3" s="70"/>
+      <c r="BG3" s="70"/>
+      <c r="BH3" s="70"/>
+      <c r="BI3" s="71"/>
+      <c r="BJ3" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="BK3" s="67"/>
-      <c r="BL3" s="67"/>
-      <c r="BM3" s="67"/>
-      <c r="BN3" s="67"/>
-      <c r="BO3" s="67"/>
-      <c r="BP3" s="68"/>
-      <c r="BQ3" s="66" t="s">
+      <c r="BK3" s="70"/>
+      <c r="BL3" s="70"/>
+      <c r="BM3" s="70"/>
+      <c r="BN3" s="70"/>
+      <c r="BO3" s="70"/>
+      <c r="BP3" s="71"/>
+      <c r="BQ3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="BR3" s="67"/>
-      <c r="BS3" s="67"/>
-      <c r="BT3" s="67"/>
-      <c r="BU3" s="67"/>
-      <c r="BV3" s="67"/>
-      <c r="BW3" s="68"/>
-      <c r="BX3" s="66" t="s">
+      <c r="BR3" s="70"/>
+      <c r="BS3" s="70"/>
+      <c r="BT3" s="70"/>
+      <c r="BU3" s="70"/>
+      <c r="BV3" s="70"/>
+      <c r="BW3" s="71"/>
+      <c r="BX3" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="BY3" s="67"/>
-      <c r="BZ3" s="67"/>
-      <c r="CA3" s="67"/>
-      <c r="CB3" s="67"/>
-      <c r="CC3" s="67"/>
-      <c r="CD3" s="68"/>
-      <c r="CE3" s="66" t="s">
+      <c r="BY3" s="70"/>
+      <c r="BZ3" s="70"/>
+      <c r="CA3" s="70"/>
+      <c r="CB3" s="70"/>
+      <c r="CC3" s="70"/>
+      <c r="CD3" s="71"/>
+      <c r="CE3" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="CF3" s="67"/>
-      <c r="CG3" s="67"/>
-      <c r="CH3" s="67"/>
-      <c r="CI3" s="67"/>
-      <c r="CJ3" s="67"/>
-      <c r="CK3" s="68"/>
-      <c r="CL3" s="66" t="s">
+      <c r="CF3" s="70"/>
+      <c r="CG3" s="70"/>
+      <c r="CH3" s="70"/>
+      <c r="CI3" s="70"/>
+      <c r="CJ3" s="70"/>
+      <c r="CK3" s="71"/>
+      <c r="CL3" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="CM3" s="67"/>
-      <c r="CN3" s="67"/>
-      <c r="CO3" s="67"/>
-      <c r="CP3" s="67"/>
-      <c r="CQ3" s="67"/>
-      <c r="CR3" s="68"/>
-      <c r="CS3" s="66" t="s">
+      <c r="CM3" s="70"/>
+      <c r="CN3" s="70"/>
+      <c r="CO3" s="70"/>
+      <c r="CP3" s="70"/>
+      <c r="CQ3" s="70"/>
+      <c r="CR3" s="71"/>
+      <c r="CS3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="CT3" s="67"/>
-      <c r="CU3" s="67"/>
-      <c r="CV3" s="67"/>
-      <c r="CW3" s="67"/>
-      <c r="CX3" s="67"/>
-      <c r="CY3" s="67"/>
-      <c r="CZ3" s="67"/>
-      <c r="DA3" s="67"/>
-      <c r="DB3" s="68"/>
-      <c r="DC3" s="66" t="s">
+      <c r="CT3" s="70"/>
+      <c r="CU3" s="70"/>
+      <c r="CV3" s="70"/>
+      <c r="CW3" s="70"/>
+      <c r="CX3" s="70"/>
+      <c r="CY3" s="70"/>
+      <c r="CZ3" s="70"/>
+      <c r="DA3" s="70"/>
+      <c r="DB3" s="71"/>
+      <c r="DC3" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="DD3" s="67"/>
-      <c r="DE3" s="67"/>
-      <c r="DF3" s="67"/>
-      <c r="DG3" s="67"/>
-      <c r="DH3" s="67"/>
-      <c r="DI3" s="67"/>
-      <c r="DJ3" s="67"/>
-      <c r="DK3" s="67"/>
-      <c r="DL3" s="67"/>
-      <c r="DM3" s="68"/>
+      <c r="DD3" s="70"/>
+      <c r="DE3" s="70"/>
+      <c r="DF3" s="70"/>
+      <c r="DG3" s="70"/>
+      <c r="DH3" s="70"/>
+      <c r="DI3" s="70"/>
+      <c r="DJ3" s="70"/>
+      <c r="DK3" s="70"/>
+      <c r="DL3" s="70"/>
+      <c r="DM3" s="71"/>
     </row>
     <row r="4" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
@@ -2245,10 +2245,10 @@
       <c r="C6" s="4"/>
       <c r="D6" s="1"/>
       <c r="E6" s="5"/>
-      <c r="I6" s="71" t="s">
+      <c r="I6" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="71"/>
+      <c r="J6" s="66"/>
       <c r="L6" t="s">
         <v>39</v>
       </c>
@@ -5858,6 +5858,9 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O1:EF1"/>
+    <mergeCell ref="DC3:DM3"/>
+    <mergeCell ref="DC2:DM2"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="CE3:CK3"/>
@@ -5873,9 +5876,6 @@
     <mergeCell ref="AC3:AI3"/>
     <mergeCell ref="AJ3:AS3"/>
     <mergeCell ref="AC2:AS2"/>
-    <mergeCell ref="O1:EF1"/>
-    <mergeCell ref="DC3:DM3"/>
-    <mergeCell ref="DC2:DM2"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:E26">
     <cfRule type="iconSet" priority="1">

</xml_diff>

<commit_message>
Asignaciones fallidas en el cronograma
</commit_message>
<xml_diff>
--- a/Documentación/Cronograma.xlsx
+++ b/Documentación/Cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\52646\Desktop\ProyectoBDITE\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3489832E-C15F-4AE3-93F9-983B838D7ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226D8E5E-CCBD-4C2A-87B6-3B469A3421E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{77C97420-D882-4AEC-80C4-94E9F25F4DD9}"/>
   </bookViews>
@@ -945,13 +945,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -963,6 +957,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -970,12 +976,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770ABD26-0474-45FB-9EFD-7F425FDDCB3A}">
   <dimension ref="A1:EF56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG8" sqref="AG8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,130 +1342,130 @@
       <c r="E1" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="75" t="s">
+      <c r="O1" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="75"/>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="75"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="75"/>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="75"/>
-      <c r="AM1" s="75"/>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="75"/>
-      <c r="AP1" s="75"/>
-      <c r="AQ1" s="75"/>
-      <c r="AR1" s="75"/>
-      <c r="AS1" s="75"/>
-      <c r="AT1" s="75"/>
-      <c r="AU1" s="75"/>
-      <c r="AV1" s="75"/>
-      <c r="AW1" s="75"/>
-      <c r="AX1" s="75"/>
-      <c r="AY1" s="75"/>
-      <c r="AZ1" s="75"/>
-      <c r="BA1" s="75"/>
-      <c r="BB1" s="75"/>
-      <c r="BC1" s="75"/>
-      <c r="BD1" s="75"/>
-      <c r="BE1" s="75"/>
-      <c r="BF1" s="75"/>
-      <c r="BG1" s="75"/>
-      <c r="BH1" s="75"/>
-      <c r="BI1" s="75"/>
-      <c r="BJ1" s="75"/>
-      <c r="BK1" s="75"/>
-      <c r="BL1" s="75"/>
-      <c r="BM1" s="75"/>
-      <c r="BN1" s="75"/>
-      <c r="BO1" s="75"/>
-      <c r="BP1" s="75"/>
-      <c r="BQ1" s="75"/>
-      <c r="BR1" s="75"/>
-      <c r="BS1" s="75"/>
-      <c r="BT1" s="75"/>
-      <c r="BU1" s="75"/>
-      <c r="BV1" s="75"/>
-      <c r="BW1" s="75"/>
-      <c r="BX1" s="75"/>
-      <c r="BY1" s="75"/>
-      <c r="BZ1" s="75"/>
-      <c r="CA1" s="75"/>
-      <c r="CB1" s="75"/>
-      <c r="CC1" s="75"/>
-      <c r="CD1" s="75"/>
-      <c r="CE1" s="75"/>
-      <c r="CF1" s="75"/>
-      <c r="CG1" s="75"/>
-      <c r="CH1" s="75"/>
-      <c r="CI1" s="75"/>
-      <c r="CJ1" s="75"/>
-      <c r="CK1" s="75"/>
-      <c r="CL1" s="75"/>
-      <c r="CM1" s="75"/>
-      <c r="CN1" s="75"/>
-      <c r="CO1" s="75"/>
-      <c r="CP1" s="75"/>
-      <c r="CQ1" s="75"/>
-      <c r="CR1" s="75"/>
-      <c r="CS1" s="75"/>
-      <c r="CT1" s="75"/>
-      <c r="CU1" s="75"/>
-      <c r="CV1" s="75"/>
-      <c r="CW1" s="75"/>
-      <c r="CX1" s="75"/>
-      <c r="CY1" s="75"/>
-      <c r="CZ1" s="75"/>
-      <c r="DA1" s="75"/>
-      <c r="DB1" s="75"/>
-      <c r="DC1" s="75"/>
-      <c r="DD1" s="75"/>
-      <c r="DE1" s="75"/>
-      <c r="DF1" s="75"/>
-      <c r="DG1" s="75"/>
-      <c r="DH1" s="75"/>
-      <c r="DI1" s="75"/>
-      <c r="DJ1" s="75"/>
-      <c r="DK1" s="75"/>
-      <c r="DL1" s="75"/>
-      <c r="DM1" s="75"/>
-      <c r="DN1" s="75"/>
-      <c r="DO1" s="75"/>
-      <c r="DP1" s="75"/>
-      <c r="DQ1" s="75"/>
-      <c r="DR1" s="75"/>
-      <c r="DS1" s="75"/>
-      <c r="DT1" s="75"/>
-      <c r="DU1" s="75"/>
-      <c r="DV1" s="75"/>
-      <c r="DW1" s="75"/>
-      <c r="DX1" s="75"/>
-      <c r="DY1" s="75"/>
-      <c r="DZ1" s="75"/>
-      <c r="EA1" s="75"/>
-      <c r="EB1" s="75"/>
-      <c r="EC1" s="75"/>
-      <c r="ED1" s="75"/>
-      <c r="EE1" s="75"/>
-      <c r="EF1" s="75"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="66"/>
+      <c r="AV1" s="66"/>
+      <c r="AW1" s="66"/>
+      <c r="AX1" s="66"/>
+      <c r="AY1" s="66"/>
+      <c r="AZ1" s="66"/>
+      <c r="BA1" s="66"/>
+      <c r="BB1" s="66"/>
+      <c r="BC1" s="66"/>
+      <c r="BD1" s="66"/>
+      <c r="BE1" s="66"/>
+      <c r="BF1" s="66"/>
+      <c r="BG1" s="66"/>
+      <c r="BH1" s="66"/>
+      <c r="BI1" s="66"/>
+      <c r="BJ1" s="66"/>
+      <c r="BK1" s="66"/>
+      <c r="BL1" s="66"/>
+      <c r="BM1" s="66"/>
+      <c r="BN1" s="66"/>
+      <c r="BO1" s="66"/>
+      <c r="BP1" s="66"/>
+      <c r="BQ1" s="66"/>
+      <c r="BR1" s="66"/>
+      <c r="BS1" s="66"/>
+      <c r="BT1" s="66"/>
+      <c r="BU1" s="66"/>
+      <c r="BV1" s="66"/>
+      <c r="BW1" s="66"/>
+      <c r="BX1" s="66"/>
+      <c r="BY1" s="66"/>
+      <c r="BZ1" s="66"/>
+      <c r="CA1" s="66"/>
+      <c r="CB1" s="66"/>
+      <c r="CC1" s="66"/>
+      <c r="CD1" s="66"/>
+      <c r="CE1" s="66"/>
+      <c r="CF1" s="66"/>
+      <c r="CG1" s="66"/>
+      <c r="CH1" s="66"/>
+      <c r="CI1" s="66"/>
+      <c r="CJ1" s="66"/>
+      <c r="CK1" s="66"/>
+      <c r="CL1" s="66"/>
+      <c r="CM1" s="66"/>
+      <c r="CN1" s="66"/>
+      <c r="CO1" s="66"/>
+      <c r="CP1" s="66"/>
+      <c r="CQ1" s="66"/>
+      <c r="CR1" s="66"/>
+      <c r="CS1" s="66"/>
+      <c r="CT1" s="66"/>
+      <c r="CU1" s="66"/>
+      <c r="CV1" s="66"/>
+      <c r="CW1" s="66"/>
+      <c r="CX1" s="66"/>
+      <c r="CY1" s="66"/>
+      <c r="CZ1" s="66"/>
+      <c r="DA1" s="66"/>
+      <c r="DB1" s="66"/>
+      <c r="DC1" s="66"/>
+      <c r="DD1" s="66"/>
+      <c r="DE1" s="66"/>
+      <c r="DF1" s="66"/>
+      <c r="DG1" s="66"/>
+      <c r="DH1" s="66"/>
+      <c r="DI1" s="66"/>
+      <c r="DJ1" s="66"/>
+      <c r="DK1" s="66"/>
+      <c r="DL1" s="66"/>
+      <c r="DM1" s="66"/>
+      <c r="DN1" s="66"/>
+      <c r="DO1" s="66"/>
+      <c r="DP1" s="66"/>
+      <c r="DQ1" s="66"/>
+      <c r="DR1" s="66"/>
+      <c r="DS1" s="66"/>
+      <c r="DT1" s="66"/>
+      <c r="DU1" s="66"/>
+      <c r="DV1" s="66"/>
+      <c r="DW1" s="66"/>
+      <c r="DX1" s="66"/>
+      <c r="DY1" s="66"/>
+      <c r="DZ1" s="66"/>
+      <c r="EA1" s="66"/>
+      <c r="EB1" s="66"/>
+      <c r="EC1" s="66"/>
+      <c r="ED1" s="66"/>
+      <c r="EE1" s="66"/>
+      <c r="EF1" s="66"/>
     </row>
     <row r="2" spans="1:136" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
@@ -1475,109 +1475,111 @@
         <v>18</v>
       </c>
       <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
       <c r="E2" s="11"/>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="68"/>
-      <c r="AC2" s="74" t="s">
+      <c r="J2" s="73"/>
+      <c r="AC2" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="AD2" s="74"/>
-      <c r="AE2" s="74"/>
-      <c r="AF2" s="74"/>
-      <c r="AG2" s="74"/>
-      <c r="AH2" s="74"/>
-      <c r="AI2" s="74"/>
-      <c r="AJ2" s="74"/>
-      <c r="AK2" s="74"/>
-      <c r="AL2" s="74"/>
-      <c r="AM2" s="74"/>
-      <c r="AN2" s="74"/>
-      <c r="AO2" s="74"/>
-      <c r="AP2" s="74"/>
-      <c r="AQ2" s="74"/>
-      <c r="AR2" s="74"/>
-      <c r="AS2" s="74"/>
-      <c r="AT2" s="72" t="s">
+      <c r="AD2" s="76"/>
+      <c r="AE2" s="76"/>
+      <c r="AF2" s="76"/>
+      <c r="AG2" s="76"/>
+      <c r="AH2" s="76"/>
+      <c r="AI2" s="76"/>
+      <c r="AJ2" s="76"/>
+      <c r="AK2" s="76"/>
+      <c r="AL2" s="76"/>
+      <c r="AM2" s="76"/>
+      <c r="AN2" s="76"/>
+      <c r="AO2" s="76"/>
+      <c r="AP2" s="76"/>
+      <c r="AQ2" s="76"/>
+      <c r="AR2" s="76"/>
+      <c r="AS2" s="76"/>
+      <c r="AT2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="AU2" s="72"/>
-      <c r="AV2" s="72"/>
-      <c r="AW2" s="72"/>
-      <c r="AX2" s="72"/>
-      <c r="AY2" s="72"/>
-      <c r="AZ2" s="72"/>
-      <c r="BA2" s="72"/>
-      <c r="BB2" s="72"/>
-      <c r="BC2" s="72"/>
-      <c r="BD2" s="72"/>
-      <c r="BE2" s="72"/>
-      <c r="BF2" s="72"/>
-      <c r="BG2" s="72"/>
-      <c r="BH2" s="72"/>
-      <c r="BI2" s="72"/>
-      <c r="BJ2" s="72"/>
-      <c r="BK2" s="72"/>
-      <c r="BL2" s="72"/>
-      <c r="BM2" s="72"/>
-      <c r="BN2" s="72"/>
-      <c r="BO2" s="72"/>
-      <c r="BP2" s="72"/>
-      <c r="BQ2" s="72"/>
-      <c r="BR2" s="72"/>
-      <c r="BS2" s="72"/>
-      <c r="BT2" s="72"/>
-      <c r="BU2" s="72"/>
-      <c r="BV2" s="72"/>
-      <c r="BW2" s="72"/>
-      <c r="BX2" s="73" t="s">
+      <c r="AU2" s="74"/>
+      <c r="AV2" s="74"/>
+      <c r="AW2" s="74"/>
+      <c r="AX2" s="74"/>
+      <c r="AY2" s="74"/>
+      <c r="AZ2" s="74"/>
+      <c r="BA2" s="74"/>
+      <c r="BB2" s="74"/>
+      <c r="BC2" s="74"/>
+      <c r="BD2" s="74"/>
+      <c r="BE2" s="74"/>
+      <c r="BF2" s="74"/>
+      <c r="BG2" s="74"/>
+      <c r="BH2" s="74"/>
+      <c r="BI2" s="74"/>
+      <c r="BJ2" s="74"/>
+      <c r="BK2" s="74"/>
+      <c r="BL2" s="74"/>
+      <c r="BM2" s="74"/>
+      <c r="BN2" s="74"/>
+      <c r="BO2" s="74"/>
+      <c r="BP2" s="74"/>
+      <c r="BQ2" s="74"/>
+      <c r="BR2" s="74"/>
+      <c r="BS2" s="74"/>
+      <c r="BT2" s="74"/>
+      <c r="BU2" s="74"/>
+      <c r="BV2" s="74"/>
+      <c r="BW2" s="74"/>
+      <c r="BX2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="BY2" s="73"/>
-      <c r="BZ2" s="73"/>
-      <c r="CA2" s="73"/>
-      <c r="CB2" s="73"/>
-      <c r="CC2" s="73"/>
-      <c r="CD2" s="73"/>
-      <c r="CE2" s="73"/>
-      <c r="CF2" s="73"/>
-      <c r="CG2" s="73"/>
-      <c r="CH2" s="73"/>
-      <c r="CI2" s="73"/>
-      <c r="CJ2" s="73"/>
-      <c r="CK2" s="73"/>
-      <c r="CL2" s="73"/>
-      <c r="CM2" s="73"/>
-      <c r="CN2" s="73"/>
-      <c r="CO2" s="73"/>
-      <c r="CP2" s="73"/>
-      <c r="CQ2" s="73"/>
-      <c r="CR2" s="73"/>
-      <c r="CS2" s="73"/>
-      <c r="CT2" s="73"/>
-      <c r="CU2" s="73"/>
-      <c r="CV2" s="73"/>
-      <c r="CW2" s="73"/>
-      <c r="CX2" s="73"/>
-      <c r="CY2" s="73"/>
-      <c r="CZ2" s="73"/>
-      <c r="DA2" s="73"/>
-      <c r="DB2" s="73"/>
-      <c r="DC2" s="76" t="s">
+      <c r="BY2" s="75"/>
+      <c r="BZ2" s="75"/>
+      <c r="CA2" s="75"/>
+      <c r="CB2" s="75"/>
+      <c r="CC2" s="75"/>
+      <c r="CD2" s="75"/>
+      <c r="CE2" s="75"/>
+      <c r="CF2" s="75"/>
+      <c r="CG2" s="75"/>
+      <c r="CH2" s="75"/>
+      <c r="CI2" s="75"/>
+      <c r="CJ2" s="75"/>
+      <c r="CK2" s="75"/>
+      <c r="CL2" s="75"/>
+      <c r="CM2" s="75"/>
+      <c r="CN2" s="75"/>
+      <c r="CO2" s="75"/>
+      <c r="CP2" s="75"/>
+      <c r="CQ2" s="75"/>
+      <c r="CR2" s="75"/>
+      <c r="CS2" s="75"/>
+      <c r="CT2" s="75"/>
+      <c r="CU2" s="75"/>
+      <c r="CV2" s="75"/>
+      <c r="CW2" s="75"/>
+      <c r="CX2" s="75"/>
+      <c r="CY2" s="75"/>
+      <c r="CZ2" s="75"/>
+      <c r="DA2" s="75"/>
+      <c r="DB2" s="75"/>
+      <c r="DC2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="DD2" s="76"/>
-      <c r="DE2" s="76"/>
-      <c r="DF2" s="76"/>
-      <c r="DG2" s="76"/>
-      <c r="DH2" s="76"/>
-      <c r="DI2" s="76"/>
-      <c r="DJ2" s="76"/>
-      <c r="DK2" s="76"/>
-      <c r="DL2" s="76"/>
-      <c r="DM2" s="76"/>
+      <c r="DD2" s="70"/>
+      <c r="DE2" s="70"/>
+      <c r="DF2" s="70"/>
+      <c r="DG2" s="70"/>
+      <c r="DH2" s="70"/>
+      <c r="DI2" s="70"/>
+      <c r="DJ2" s="70"/>
+      <c r="DK2" s="70"/>
+      <c r="DL2" s="70"/>
+      <c r="DM2" s="70"/>
     </row>
     <row r="3" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
@@ -1587,121 +1589,123 @@
         <v>20</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
-      <c r="AC3" s="69" t="s">
+      <c r="AC3" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="70"/>
-      <c r="AG3" s="70"/>
-      <c r="AH3" s="70"/>
-      <c r="AI3" s="71"/>
-      <c r="AJ3" s="70" t="s">
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="69"/>
+      <c r="AJ3" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="AK3" s="70"/>
-      <c r="AL3" s="70"/>
-      <c r="AM3" s="70"/>
-      <c r="AN3" s="70"/>
-      <c r="AO3" s="70"/>
-      <c r="AP3" s="70"/>
-      <c r="AQ3" s="70"/>
-      <c r="AR3" s="70"/>
-      <c r="AS3" s="71"/>
-      <c r="AT3" s="69" t="s">
+      <c r="AK3" s="68"/>
+      <c r="AL3" s="68"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="69"/>
+      <c r="AT3" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="AU3" s="70"/>
-      <c r="AV3" s="70"/>
-      <c r="AW3" s="70"/>
-      <c r="AX3" s="70"/>
-      <c r="AY3" s="70"/>
-      <c r="AZ3" s="70"/>
-      <c r="BA3" s="70"/>
-      <c r="BB3" s="71"/>
-      <c r="BC3" s="69" t="s">
+      <c r="AU3" s="68"/>
+      <c r="AV3" s="68"/>
+      <c r="AW3" s="68"/>
+      <c r="AX3" s="68"/>
+      <c r="AY3" s="68"/>
+      <c r="AZ3" s="68"/>
+      <c r="BA3" s="68"/>
+      <c r="BB3" s="69"/>
+      <c r="BC3" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="BD3" s="70"/>
-      <c r="BE3" s="70"/>
-      <c r="BF3" s="70"/>
-      <c r="BG3" s="70"/>
-      <c r="BH3" s="70"/>
-      <c r="BI3" s="71"/>
-      <c r="BJ3" s="69" t="s">
+      <c r="BD3" s="68"/>
+      <c r="BE3" s="68"/>
+      <c r="BF3" s="68"/>
+      <c r="BG3" s="68"/>
+      <c r="BH3" s="68"/>
+      <c r="BI3" s="69"/>
+      <c r="BJ3" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="BK3" s="70"/>
-      <c r="BL3" s="70"/>
-      <c r="BM3" s="70"/>
-      <c r="BN3" s="70"/>
-      <c r="BO3" s="70"/>
-      <c r="BP3" s="71"/>
-      <c r="BQ3" s="69" t="s">
+      <c r="BK3" s="68"/>
+      <c r="BL3" s="68"/>
+      <c r="BM3" s="68"/>
+      <c r="BN3" s="68"/>
+      <c r="BO3" s="68"/>
+      <c r="BP3" s="69"/>
+      <c r="BQ3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="BR3" s="70"/>
-      <c r="BS3" s="70"/>
-      <c r="BT3" s="70"/>
-      <c r="BU3" s="70"/>
-      <c r="BV3" s="70"/>
-      <c r="BW3" s="71"/>
-      <c r="BX3" s="69" t="s">
+      <c r="BR3" s="68"/>
+      <c r="BS3" s="68"/>
+      <c r="BT3" s="68"/>
+      <c r="BU3" s="68"/>
+      <c r="BV3" s="68"/>
+      <c r="BW3" s="69"/>
+      <c r="BX3" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="BY3" s="70"/>
-      <c r="BZ3" s="70"/>
-      <c r="CA3" s="70"/>
-      <c r="CB3" s="70"/>
-      <c r="CC3" s="70"/>
-      <c r="CD3" s="71"/>
-      <c r="CE3" s="69" t="s">
+      <c r="BY3" s="68"/>
+      <c r="BZ3" s="68"/>
+      <c r="CA3" s="68"/>
+      <c r="CB3" s="68"/>
+      <c r="CC3" s="68"/>
+      <c r="CD3" s="69"/>
+      <c r="CE3" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="CF3" s="70"/>
-      <c r="CG3" s="70"/>
-      <c r="CH3" s="70"/>
-      <c r="CI3" s="70"/>
-      <c r="CJ3" s="70"/>
-      <c r="CK3" s="71"/>
-      <c r="CL3" s="69" t="s">
+      <c r="CF3" s="68"/>
+      <c r="CG3" s="68"/>
+      <c r="CH3" s="68"/>
+      <c r="CI3" s="68"/>
+      <c r="CJ3" s="68"/>
+      <c r="CK3" s="69"/>
+      <c r="CL3" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="CM3" s="70"/>
-      <c r="CN3" s="70"/>
-      <c r="CO3" s="70"/>
-      <c r="CP3" s="70"/>
-      <c r="CQ3" s="70"/>
-      <c r="CR3" s="71"/>
-      <c r="CS3" s="69" t="s">
+      <c r="CM3" s="68"/>
+      <c r="CN3" s="68"/>
+      <c r="CO3" s="68"/>
+      <c r="CP3" s="68"/>
+      <c r="CQ3" s="68"/>
+      <c r="CR3" s="69"/>
+      <c r="CS3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="CT3" s="70"/>
-      <c r="CU3" s="70"/>
-      <c r="CV3" s="70"/>
-      <c r="CW3" s="70"/>
-      <c r="CX3" s="70"/>
-      <c r="CY3" s="70"/>
-      <c r="CZ3" s="70"/>
-      <c r="DA3" s="70"/>
-      <c r="DB3" s="71"/>
-      <c r="DC3" s="69" t="s">
+      <c r="CT3" s="68"/>
+      <c r="CU3" s="68"/>
+      <c r="CV3" s="68"/>
+      <c r="CW3" s="68"/>
+      <c r="CX3" s="68"/>
+      <c r="CY3" s="68"/>
+      <c r="CZ3" s="68"/>
+      <c r="DA3" s="68"/>
+      <c r="DB3" s="69"/>
+      <c r="DC3" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="DD3" s="70"/>
-      <c r="DE3" s="70"/>
-      <c r="DF3" s="70"/>
-      <c r="DG3" s="70"/>
-      <c r="DH3" s="70"/>
-      <c r="DI3" s="70"/>
-      <c r="DJ3" s="70"/>
-      <c r="DK3" s="70"/>
-      <c r="DL3" s="70"/>
-      <c r="DM3" s="71"/>
+      <c r="DD3" s="68"/>
+      <c r="DE3" s="68"/>
+      <c r="DF3" s="68"/>
+      <c r="DG3" s="68"/>
+      <c r="DH3" s="68"/>
+      <c r="DI3" s="68"/>
+      <c r="DJ3" s="68"/>
+      <c r="DK3" s="68"/>
+      <c r="DL3" s="68"/>
+      <c r="DM3" s="69"/>
     </row>
     <row r="4" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
@@ -2245,10 +2249,10 @@
       <c r="C6" s="4"/>
       <c r="D6" s="1"/>
       <c r="E6" s="5"/>
-      <c r="I6" s="66" t="s">
+      <c r="I6" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="66"/>
+      <c r="J6" s="71"/>
       <c r="L6" t="s">
         <v>39</v>
       </c>
@@ -5858,6 +5862,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AJ3:AS3"/>
+    <mergeCell ref="AC2:AS2"/>
     <mergeCell ref="O1:EF1"/>
     <mergeCell ref="DC3:DM3"/>
     <mergeCell ref="DC2:DM2"/>
@@ -5874,8 +5880,6 @@
     <mergeCell ref="BQ3:BW3"/>
     <mergeCell ref="BX3:CD3"/>
     <mergeCell ref="AC3:AI3"/>
-    <mergeCell ref="AJ3:AS3"/>
-    <mergeCell ref="AC2:AS2"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:E26">
     <cfRule type="iconSet" priority="1">

</xml_diff>